<commit_message>
add new complex data structure(not finished)
</commit_message>
<xml_diff>
--- a/bin/resource/excel/Player.xlsx
+++ b/bin/resource/excel/Player.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\opensource\ARK.net_header\Bin\resource\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="27525" windowHeight="17535" activeTab="1"/>
+    <workbookView windowWidth="27870" windowHeight="13065" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataNode_1" sheetId="1" r:id="rId1"/>
@@ -22,14 +17,6 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -39,7 +26,7 @@
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="D8" authorId="0" shapeId="0">
+    <comment ref="D8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0">
+    <comment ref="F8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -87,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0">
+    <comment ref="H8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="I8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -111,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="0" shapeId="0">
+    <comment ref="J8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -123,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K8" authorId="0" shapeId="0">
+    <comment ref="K8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116">
   <si>
     <t>Id</t>
   </si>
@@ -148,9 +135,18 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Career</t>
+  </si>
+  <si>
     <t>Camp</t>
   </si>
   <si>
+    <t>LastMapID</t>
+  </si>
+  <si>
     <t>Level</t>
   </si>
   <si>
@@ -181,9 +177,15 @@
     <t>OnlineCount</t>
   </si>
   <si>
+    <t>TotalOnlineTime</t>
+  </si>
+  <si>
     <t>LastOfflineTime</t>
   </si>
   <si>
+    <t>LoadDataFinish</t>
+  </si>
+  <si>
     <t>GameID</t>
   </si>
   <si>
@@ -223,18 +225,21 @@
     <t>性别</t>
   </si>
   <si>
+    <t>职业</t>
+  </si>
+  <si>
     <t>阵营</t>
   </si>
   <si>
+    <t>上次在线的场景</t>
+  </si>
+  <si>
     <t>等级</t>
   </si>
   <si>
     <t>角色类型</t>
   </si>
   <si>
-    <t>职业</t>
-  </si>
-  <si>
     <t>经验获得,如果是怪物，则是掉落经验</t>
   </si>
   <si>
@@ -271,6 +276,102 @@
     <t>登陆的网关ID</t>
   </si>
   <si>
+    <t>BagEquipList</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Col</t>
+  </si>
+  <si>
+    <t>GUID</t>
+  </si>
+  <si>
+    <t>WearGUID</t>
+  </si>
+  <si>
+    <t>ConfigID</t>
+  </si>
+  <si>
+    <t>ExpiredType</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>RandPropertyID</t>
+  </si>
+  <si>
+    <t>SlotCount</t>
+  </si>
+  <si>
+    <t>InlayStone1</t>
+  </si>
+  <si>
+    <t>InlayStone2</t>
+  </si>
+  <si>
+    <t>InlayStone3</t>
+  </si>
+  <si>
+    <t>InlayStone4</t>
+  </si>
+  <si>
+    <t>InlayStone5</t>
+  </si>
+  <si>
+    <t>InlayStone6</t>
+  </si>
+  <si>
+    <t>InlayStone7</t>
+  </si>
+  <si>
+    <t>InlayStone8</t>
+  </si>
+  <si>
+    <t>InlayStone9</t>
+  </si>
+  <si>
+    <t>InlayStone10</t>
+  </si>
+  <si>
+    <t>IntensifyLevel</t>
+  </si>
+  <si>
+    <t>ElementLevel1_FIRE</t>
+  </si>
+  <si>
+    <t>ElementLevel2_LIGHT</t>
+  </si>
+  <si>
+    <t>ElementLevel3_Wind</t>
+  </si>
+  <si>
+    <t>ElementLevel4_ICE</t>
+  </si>
+  <si>
+    <t>ElementLevel5_POISON</t>
+  </si>
+  <si>
+    <t>int64</t>
+  </si>
+  <si>
+    <t>普通背包</t>
+  </si>
+  <si>
+    <t>BagItemList</t>
+  </si>
+  <si>
+    <t>ItemCount</t>
+  </si>
+  <si>
+    <t>Bound</t>
+  </si>
+  <si>
+    <t>CommPropertyValue</t>
+  </si>
+  <si>
     <t>SUCKBLOOD</t>
   </si>
   <si>
@@ -358,102 +459,9 @@
     <t>BUFF_GATE</t>
   </si>
   <si>
-    <t>Row</t>
-  </si>
-  <si>
-    <t>Col</t>
-  </si>
-  <si>
-    <t>GUID</t>
-  </si>
-  <si>
-    <t>ConfigID</t>
-  </si>
-  <si>
     <t>所有和战斗，药水有关的，都在这里NPC怪物只有基础和BUFF影响，因此针对玩家和怪物，分2个表.0职业等级叠加属性,1装备属性,2永久BUFF属性,3动态BUFF属性</t>
   </si>
   <si>
-    <t>BagEquipList</t>
-  </si>
-  <si>
-    <t>WearGUID</t>
-  </si>
-  <si>
-    <t>ExpiredType</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>RandPropertyID</t>
-  </si>
-  <si>
-    <t>SlotCount</t>
-  </si>
-  <si>
-    <t>InlayStone1</t>
-  </si>
-  <si>
-    <t>InlayStone2</t>
-  </si>
-  <si>
-    <t>InlayStone3</t>
-  </si>
-  <si>
-    <t>InlayStone4</t>
-  </si>
-  <si>
-    <t>InlayStone5</t>
-  </si>
-  <si>
-    <t>InlayStone6</t>
-  </si>
-  <si>
-    <t>InlayStone7</t>
-  </si>
-  <si>
-    <t>InlayStone8</t>
-  </si>
-  <si>
-    <t>InlayStone9</t>
-  </si>
-  <si>
-    <t>InlayStone10</t>
-  </si>
-  <si>
-    <t>IntensifyLevel</t>
-  </si>
-  <si>
-    <t>ElementLevel1_FIRE</t>
-  </si>
-  <si>
-    <t>ElementLevel2_LIGHT</t>
-  </si>
-  <si>
-    <t>ElementLevel3_Wind</t>
-  </si>
-  <si>
-    <t>ElementLevel4_ICE</t>
-  </si>
-  <si>
-    <t>ElementLevel5_POISON</t>
-  </si>
-  <si>
-    <t>普通背包</t>
-  </si>
-  <si>
-    <t>BagItemList</t>
-  </si>
-  <si>
-    <t>ItemCount</t>
-  </si>
-  <si>
-    <t>Bound</t>
-  </si>
-  <si>
-    <t>CommPropertyValue</t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -467,44 +475,19 @@
   </si>
   <si>
     <t>测试组件</t>
-  </si>
-  <si>
-    <t>LastMapID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gender</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Career</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上次在线的场景</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TotalOnlineTime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LoadDataFinish</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int64</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -512,20 +495,352 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -533,9 +848,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -547,13 +1104,61 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -576,9 +1181,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -907,39 +1509,40 @@
       <a:lstStyle/>
     </a:spDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I32" sqref="I32"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8:R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
     <col min="2" max="2" width="8.125" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="8.125" customWidth="1"/>
-    <col min="6" max="6" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.125" customWidth="1"/>
     <col min="7" max="7" width="9.375" customWidth="1"/>
     <col min="8" max="8" width="17.375" customWidth="1"/>
-    <col min="15" max="15" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.5" customWidth="1"/>
+    <col min="16" max="16" width="12.75" customWidth="1"/>
+    <col min="17" max="18" width="17.25" customWidth="1"/>
+    <col min="19" max="19" width="20.5" customWidth="1"/>
+    <col min="20" max="20" width="11.125" customWidth="1"/>
+    <col min="21" max="21" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -947,131 +1550,131 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>109</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="O2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="R2" t="s">
-        <v>116</v>
+        <v>23</v>
       </c>
       <c r="S2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="T2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="U2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1134,9 +1737,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1199,9 +1802,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1264,9 +1867,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -1329,9 +1932,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -1394,92 +1997,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>112</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J8" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="K8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="M8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="N8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="O8" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="P8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="Q8" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="R8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="T8" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="U8" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="A18" sqref="A18:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12.625" customWidth="1"/>
     <col min="2" max="2" width="15.375" customWidth="1"/>
     <col min="3" max="3" width="10.375" customWidth="1"/>
     <col min="4" max="4" width="14.125" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="6" max="6" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.25" customWidth="1"/>
     <col min="11" max="11" width="12.625" customWidth="1"/>
     <col min="12" max="12" width="16.5" customWidth="1"/>
     <col min="13" max="13" width="8.375" customWidth="1"/>
@@ -1490,331 +2093,331 @@
     <col min="27" max="31" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B2">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" t="s">
+        <v>63</v>
+      </c>
+      <c r="M8" t="s">
+        <v>64</v>
+      </c>
+      <c r="N8" t="s">
+        <v>65</v>
+      </c>
+      <c r="O8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>68</v>
+      </c>
+      <c r="R8" t="s">
+        <v>69</v>
+      </c>
+      <c r="S8" t="s">
+        <v>70</v>
+      </c>
+      <c r="T8" t="s">
+        <v>71</v>
+      </c>
+      <c r="U8" t="s">
+        <v>72</v>
+      </c>
+      <c r="V8" t="s">
         <v>73</v>
       </c>
-      <c r="B3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+      <c r="W8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8" t="s">
-        <v>82</v>
-      </c>
-      <c r="H8" t="s">
-        <v>83</v>
-      </c>
-      <c r="I8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" t="s">
-        <v>85</v>
-      </c>
-      <c r="K8" t="s">
-        <v>86</v>
-      </c>
-      <c r="L8" t="s">
-        <v>87</v>
-      </c>
-      <c r="M8" t="s">
-        <v>88</v>
-      </c>
-      <c r="N8" t="s">
-        <v>89</v>
-      </c>
-      <c r="O8" t="s">
-        <v>90</v>
-      </c>
-      <c r="P8" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>92</v>
-      </c>
-      <c r="R8" t="s">
-        <v>93</v>
-      </c>
-      <c r="S8" t="s">
-        <v>94</v>
-      </c>
-      <c r="T8" t="s">
-        <v>95</v>
-      </c>
-      <c r="U8" t="s">
-        <v>96</v>
-      </c>
-      <c r="V8" t="s">
-        <v>97</v>
-      </c>
-      <c r="W8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="L9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="M9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="N9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="O9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="P9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="Q9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="R9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="S9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="T9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="U9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="V9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="W9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A8" sqref="A8:AC8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="19.375" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
     <col min="8" max="9" width="9.125" customWidth="1"/>
@@ -1841,302 +2444,301 @@
     <col min="35" max="35" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B2">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B3">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="J8" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="K8" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="L8" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="M8" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="N8" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="O8" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="P8" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="Q8" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="R8" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="S8" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="T8" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="U8" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="V8" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="W8" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="X8" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="Y8" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="Z8" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="AA8" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="AB8" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="AC8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="M9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="O9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="P9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="Q9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="R9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="S9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="T9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="U9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="V9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="W9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="X9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="Y9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="Z9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="AA9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="AB9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="AC9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="8.125" customWidth="1"/>
     <col min="2" max="2" width="12.625" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"lua,python,C#,js"</formula1>
@@ -2145,7 +2747,7 @@
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>